<commit_message>
ICE-PCBA und JTag stecker hinzugefügt
</commit_message>
<xml_diff>
--- a/BOM/materialliste_microcontroller_board.xlsx
+++ b/BOM/materialliste_microcontroller_board.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studmswch-my.sharepoint.com/personal/dario_duendar_msw_ch/Documents/Atmel/uC-Boards/MC-Boards/Materialliste/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uC_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{6D3D28C0-6A12-4AA0-B1DD-35E8A2691E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9F9F9F48-035F-4E8C-BA32-1A0D6683B691}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41041325-9362-4F83-852A-BFAAE892C64E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="-120" windowWidth="27675" windowHeight="16440" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
+    <workbookView xWindow="1245" yWindow="-120" windowWidth="37275" windowHeight="21840" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Altes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="206">
   <si>
     <t>Anzahl Boards:</t>
   </si>
@@ -649,6 +648,45 @@
   <si>
     <t xml:space="preserve">667-ERB-RG2R00V </t>
   </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>Atmel-Ice-Pcba</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>https://ch.farnell.com/microchip/atatmel-ice-pcba/debugger-atmel-arm-avr-pcba-kit/dp/2407171</t>
+  </si>
+  <si>
+    <t>Jtag stecker</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 10POS IDC GOLD</t>
+  </si>
+  <si>
+    <t>1175-1646-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/products/de?keywords=1175-1646</t>
+  </si>
+  <si>
+    <t>FLAT RBN CBL GRAY 10 COND 100'</t>
+  </si>
+  <si>
+    <t>CN211GR-100-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/products/de?keywords=cn211gr-100</t>
+  </si>
+  <si>
+    <t>Jtag Kabel ca 10 cm</t>
+  </si>
+  <si>
+    <t>Nicht Bestellen Klassensatz</t>
+  </si>
 </sst>
 </file>
 
@@ -976,7 +1014,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -988,6 +1026,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1086,6 +1131,13 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1415,9 +1467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67FD4D50-7A26-44A2-B50E-5F0DC5FBBEB7}">
   <dimension ref="A1:O999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,8 +1574,8 @@
         <f>IF(OR(L2="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L2)</f>
         <v>11.200000000000001</v>
       </c>
-      <c r="O2" s="22" t="s">
-        <v>186</v>
+      <c r="O2" s="10" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1565,7 +1617,7 @@
         <v>579.95000000000005</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1607,7 +1659,7 @@
         <v>15.925000000000001</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1649,7 +1701,7 @@
         <v>2.4849999999999999</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1691,7 +1743,7 @@
         <v>10.324999999999999</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1731,7 +1783,7 @@
         <v>1149.05</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2480,7 +2532,7 @@
         <v>33.25</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2522,7 +2574,7 @@
         <v>147</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2858,7 +2910,7 @@
         <v>13.125</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -3154,7 +3206,7 @@
         <v>38.64</v>
       </c>
       <c r="O41" s="10" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -3368,92 +3420,141 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="30" t="str">
+      <c r="D47" s="8">
+        <v>1</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H47" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47">
+        <v>2407171</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="K47" s="12">
+        <v>55.64</v>
+      </c>
+      <c r="L47" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M47" s="31" t="str">
+        <v>55.64</v>
+      </c>
+      <c r="M47" s="31">
         <f>IF(OR(D47="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D47)</f>
-        <v/>
-      </c>
-      <c r="N47" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N47" s="30">
         <f>IF(OR(L47="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L47)</f>
-        <v/>
-      </c>
-      <c r="O47" s="10"/>
+        <v>1947.4</v>
+      </c>
+      <c r="O47" s="10" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="16"/>
+      <c r="D48" s="8">
+        <v>2</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>198</v>
+      </c>
       <c r="G48" s="17"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="30" t="str">
+      <c r="H48" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="I48" t="s">
+        <v>199</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="K48" s="18">
+        <v>1</v>
+      </c>
+      <c r="L48" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M48" s="31" t="str">
+        <v>2</v>
+      </c>
+      <c r="M48" s="31">
         <f>IF(OR(D48="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D48)</f>
-        <v/>
-      </c>
-      <c r="N48" s="30" t="str">
+        <v>70</v>
+      </c>
+      <c r="N48" s="30">
         <f>IF(OR(L48="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L48)</f>
-        <v/>
-      </c>
-      <c r="O48" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="13"/>
+      <c r="D49" s="8">
+        <v>1</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" t="s">
+        <v>201</v>
+      </c>
       <c r="G49" s="10"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="30" t="str">
+      <c r="H49" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="I49" t="s">
+        <v>202</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="K49" s="12">
+        <f>33/30.8*0.1</f>
+        <v>0.10714285714285715</v>
+      </c>
+      <c r="L49" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M49" s="31" t="str">
+        <v>0.10714285714285715</v>
+      </c>
+      <c r="M49" s="31">
         <f>IF(OR(D49="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D49)</f>
-        <v/>
-      </c>
-      <c r="N49" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N49" s="30">
         <f>IF(OR(L49="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L49)</f>
-        <v/>
-      </c>
-      <c r="O49" s="10"/>
+        <v>3.7500000000000004</v>
+      </c>
+      <c r="O49" s="10" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
-        <v>175</v>
-      </c>
+      <c r="A50" s="33"/>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
       <c r="D50" s="8"/>
@@ -3479,9 +3580,7 @@
       <c r="O50" s="10"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="33" t="s">
-        <v>178</v>
-      </c>
+      <c r="A51" s="33"/>
       <c r="B51" s="33"/>
       <c r="C51" s="33"/>
       <c r="D51" s="8"/>
@@ -3507,9 +3606,7 @@
       <c r="O51" s="10"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="33" t="s">
-        <v>175</v>
-      </c>
+      <c r="A52" s="33"/>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
       <c r="D52" s="8"/>
@@ -3535,9 +3632,7 @@
       <c r="O52" s="10"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A53" s="33"/>
       <c r="B53" s="33"/>
       <c r="C53" s="33"/>
       <c r="D53" s="8"/>
@@ -3563,9 +3658,7 @@
       <c r="O53" s="10"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A54" s="33"/>
       <c r="B54" s="33"/>
       <c r="C54" s="33"/>
       <c r="D54" s="8"/>
@@ -3591,9 +3684,7 @@
       <c r="O54" s="10"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A55" s="33"/>
       <c r="B55" s="33"/>
       <c r="C55" s="33"/>
       <c r="D55" s="8"/>
@@ -3619,9 +3710,7 @@
       <c r="O55" s="10"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A56" s="33"/>
       <c r="B56" s="33"/>
       <c r="C56" s="33"/>
       <c r="D56" s="8"/>
@@ -3647,9 +3736,7 @@
       <c r="O56" s="10"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
-        <v>184</v>
-      </c>
+      <c r="A57" s="33"/>
       <c r="B57" s="33"/>
       <c r="C57" s="33"/>
       <c r="D57" s="8"/>
@@ -27191,7 +27278,7 @@
       <c r="J962" s="33"/>
       <c r="K962" s="12"/>
       <c r="L962" s="30" t="str">
-        <f t="shared" ref="L962:L1025" si="15">IF(OR(K962=0,D962=0),"",D962*K962)</f>
+        <f t="shared" ref="L962:L999" si="15">IF(OR(K962=0,D962=0),"",D962*K962)</f>
         <v/>
       </c>
       <c r="M962" s="31" t="str">
@@ -28170,43 +28257,35 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O999">
     <sortCondition ref="D1:D999"/>
   </sortState>
-  <conditionalFormatting sqref="A2:B5 A13:B999 A7:B11">
-    <cfRule type="expression" dxfId="17" priority="9">
+  <conditionalFormatting sqref="A2:B5 A7:B11 A13:B999">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>(ISBLANK(A2)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O5 O13:O999 O7:O11">
-    <cfRule type="notContainsText" dxfId="16" priority="7" operator="notContains" text="ok">
+  <conditionalFormatting sqref="O2:O11 O13:O999">
+    <cfRule type="notContainsText" dxfId="3" priority="7" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="18" priority="6">
       <formula>(ISBLANK(A12)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="notContainsText" dxfId="13" priority="4" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="17" priority="4" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O12))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>(ISBLANK(A6)=FALSE)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O6">
-    <cfRule type="notContainsText" dxfId="10" priority="1" operator="notContains" text="ok">
-      <formula>ISERROR(SEARCH("ok",O6))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="ok">
-      <formula>NOT(ISERROR(SEARCH("ok",O6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -28248,7 +28327,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(Stückliste!L2:L999)</f>
-        <v>90.139000000000024</v>
+        <v>147.88614285714289</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -28258,7 +28337,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUM(Stückliste!N2:N999)</f>
-        <v>3154.8650000000002</v>
+        <v>5176.0150000000003</v>
       </c>
     </row>
   </sheetData>
@@ -53577,7 +53656,7 @@
       <c r="J962" s="33"/>
       <c r="K962" s="12"/>
       <c r="L962" s="30" t="str">
-        <f t="shared" ref="L962:L1025" si="15">IF(OR(K962=0,D962=0),"",D962*K962)</f>
+        <f t="shared" ref="L962:L999" si="15">IF(OR(K962=0,D962=0),"",D962*K962)</f>
         <v/>
       </c>
       <c r="M962" s="31" t="str">
@@ -54554,41 +54633,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B5 A13:B999 A7:B11">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>(ISBLANK(A2)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O5 O13:O999 O7:O11">
-    <cfRule type="notContainsText" dxfId="7" priority="7" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="11" priority="7" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>(ISBLANK(A12)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="8" priority="4" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O12))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>(ISBLANK(A6)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="notContainsText" dxfId="1" priority="1" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="5" priority="1" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O6))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O6)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Micro USB für JTAG hinzugefügt
</commit_message>
<xml_diff>
--- a/BOM/materialliste_microcontroller_board.xlsx
+++ b/BOM/materialliste_microcontroller_board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uC_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1781C224-1CE9-4208-828C-F2DB6EFDF917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030A9321-C704-4EAA-B1C5-ED0834467165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="-120" windowWidth="27675" windowHeight="16440" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
+    <workbookView xWindow="1260" yWindow="-108" windowWidth="21888" windowHeight="13176" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="210">
   <si>
     <t>Anzahl Boards:</t>
   </si>
@@ -686,6 +686,18 @@
   </si>
   <si>
     <t>https://www.digikey.ch/product-detail/de/3230-10-0102-00/3230-10-0102-00-ND/3883464/?itemSeq=343224426</t>
+  </si>
+  <si>
+    <t>Micro-USB für Jtag</t>
+  </si>
+  <si>
+    <t>RND 765-00054 - USB-A Micro-B</t>
+  </si>
+  <si>
+    <t>301-25-772</t>
+  </si>
+  <si>
+    <t>https://www.distrelec.ch/de/usb-anschluss-auf-usb-micro-anschlusskabel-900mm-schwarz-rnd-connect-rnd-765-00054/p/30125772</t>
   </si>
 </sst>
 </file>
@@ -1440,8 +1452,8 @@
   <dimension ref="A1:O999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I53" sqref="I53"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3526,30 +3538,48 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="33"/>
+      <c r="A50" s="33" t="s">
+        <v>203</v>
+      </c>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="13"/>
+      <c r="D50" s="8">
+        <v>1</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" t="s">
+        <v>207</v>
+      </c>
       <c r="G50" s="10"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="30" t="str">
+      <c r="H50" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="K50" s="12">
+        <v>1.24</v>
+      </c>
+      <c r="L50" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M50" s="31" t="str">
+        <v>1.24</v>
+      </c>
+      <c r="M50" s="31">
         <f>IF(OR(D50="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D50)</f>
-        <v/>
-      </c>
-      <c r="N50" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N50" s="30">
         <f>IF(OR(L50="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L50)</f>
-        <v/>
-      </c>
-      <c r="O50" s="10"/>
+        <v>43.4</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="33"/>
@@ -28299,7 +28329,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(Stückliste!L2:L999)</f>
-        <v>147.26614285714288</v>
+        <v>148.50614285714289</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -28309,7 +28339,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUM(Stückliste!N2:N999)</f>
-        <v>5154.3150000000005</v>
+        <v>5197.7150000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update für version 2021 (EK20)
</commit_message>
<xml_diff>
--- a/BOM/materialliste_microcontroller_board.xlsx
+++ b/BOM/materialliste_microcontroller_board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uC_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030A9321-C704-4EAA-B1C5-ED0834467165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541E5FE-EBCA-4949-856E-3E0614B1609D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-108" windowWidth="21888" windowHeight="13176" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Altes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="217">
   <si>
     <t>Anzahl Boards:</t>
   </si>
@@ -598,19 +599,7 @@
     <t>nicht bestellen</t>
   </si>
   <si>
-    <t>40/70</t>
-  </si>
-  <si>
-    <t>15/35</t>
-  </si>
-  <si>
     <t>nicht bestücken</t>
-  </si>
-  <si>
-    <t>40/105</t>
-  </si>
-  <si>
-    <t>30/35</t>
   </si>
   <si>
     <t>Joystick</t>
@@ -626,18 +615,6 @@
   </si>
   <si>
     <t>red</t>
-  </si>
-  <si>
-    <t>0/35</t>
-  </si>
-  <si>
-    <t>0/70</t>
-  </si>
-  <si>
-    <t>0/280</t>
-  </si>
-  <si>
-    <t>10/35</t>
   </si>
   <si>
     <t xml:space="preserve">200-MMS10902FSV </t>
@@ -698,6 +675,51 @@
   </si>
   <si>
     <t>https://www.distrelec.ch/de/usb-anschluss-auf-usb-micro-anschlusskabel-900mm-schwarz-rnd-connect-rnd-765-00054/p/30125772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">695-HCM49-16MABKUT </t>
+  </si>
+  <si>
+    <t>20, 150 bestellt</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>100uF  16V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-CR1206FX-1500ELF </t>
+  </si>
+  <si>
+    <t>20, 50 bestellt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFH 5701 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">720-SFH5701 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-DMG3406L-13 </t>
+  </si>
+  <si>
+    <t>ATMEGA2560-16AU-ND</t>
+  </si>
+  <si>
+    <t>10, 50 bestellt</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-74HC14D-Q100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-3314R-GM5-503E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">710-865230245004 </t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1048,175 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1452,8 +1642,8 @@
   <dimension ref="A1:O999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1658,7 @@
     <col min="10" max="10" width="8.5703125" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" style="19" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="37"/>
+    <col min="15" max="15" width="19.5703125" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1537,10 +1727,10 @@
         <v>152</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" s="21">
-        <v>17390099</v>
+        <v>213</v>
+      </c>
+      <c r="I2" t="s">
+        <v>214</v>
       </c>
       <c r="J2" s="29"/>
       <c r="K2" s="23">
@@ -1579,10 +1769,10 @@
         <v>51</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>52</v>
+        <v>140</v>
+      </c>
+      <c r="I3" t="s">
+        <v>211</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="12">
@@ -1707,16 +1897,16 @@
       <c r="H6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>56</v>
+      <c r="I6" t="s">
+        <v>202</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="12">
-        <v>0.29499999999999998</v>
+        <v>0.46</v>
       </c>
       <c r="L6" s="30">
         <f t="shared" si="0"/>
-        <v>0.29499999999999998</v>
+        <v>0.46</v>
       </c>
       <c r="M6" s="31">
         <f>IF(OR(D6="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D6)</f>
@@ -1724,7 +1914,7 @@
       </c>
       <c r="N6" s="30">
         <f>IF(OR(L6="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L6)</f>
-        <v>10.324999999999999</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="O6" s="10" t="s">
         <v>173</v>
@@ -1905,22 +2095,22 @@
         <v>143</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>144</v>
+        <v>208</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="I11" s="9">
-        <v>632917</v>
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>209</v>
       </c>
       <c r="J11" s="33"/>
       <c r="K11" s="12">
-        <v>0.879</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="L11" s="30">
         <f t="shared" si="0"/>
-        <v>0.879</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="M11" s="31">
         <f>IF(OR(D11="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D11)</f>
@@ -1928,7 +2118,7 @@
       </c>
       <c r="N11" s="30">
         <f>IF(OR(L11="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L11)</f>
-        <v>30.765000000000001</v>
+        <v>21.524999999999999</v>
       </c>
       <c r="O11" s="10" t="s">
         <v>173</v>
@@ -2059,11 +2249,13 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+      <c r="A15" s="33" t="s">
+        <v>176</v>
+      </c>
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
       <c r="D15" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>121</v>
@@ -2084,28 +2276,30 @@
       <c r="K15" s="12">
         <v>0.70199999999999996</v>
       </c>
-      <c r="L15" s="30">
+      <c r="L15" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>0.70199999999999996</v>
+        <v/>
       </c>
       <c r="M15" s="31">
         <f>IF(OR(D15="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D15)</f>
-        <v>35</v>
-      </c>
-      <c r="N15" s="30">
+        <v>0</v>
+      </c>
+      <c r="N15" s="30" t="str">
         <f>IF(OR(L15="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L15)</f>
-        <v>24.57</v>
+        <v/>
       </c>
       <c r="O15" s="10" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+      <c r="A16" s="33" t="s">
+        <v>176</v>
+      </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
       <c r="D16" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>124</v>
@@ -2126,17 +2320,17 @@
       <c r="K16" s="12">
         <v>2.6</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>2.6</v>
+        <v/>
       </c>
       <c r="M16" s="31">
         <f>IF(OR(D16="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D16)</f>
-        <v>35</v>
-      </c>
-      <c r="N16" s="30">
+        <v>0</v>
+      </c>
+      <c r="N16" s="30" t="str">
         <f>IF(OR(L16="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L16)</f>
-        <v>91</v>
+        <v/>
       </c>
       <c r="O16" s="10" t="s">
         <v>173</v>
@@ -2287,8 +2481,8 @@
       <c r="H20" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>88</v>
+      <c r="I20" t="s">
+        <v>215</v>
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="12">
@@ -2444,10 +2638,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="33" t="s">
@@ -2455,7 +2649,7 @@
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="35" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K24" s="18">
         <f>(1.7+1.82)/2</f>
@@ -2488,7 +2682,7 @@
         <v>125</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G25" s="9">
         <v>1206</v>
@@ -2497,7 +2691,7 @@
         <v>18</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="12">
@@ -2539,7 +2733,7 @@
         <v>18</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="J26" s="11"/>
       <c r="K26" s="18">
@@ -2866,7 +3060,7 @@
         <v>32</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>33</v>
+        <v>205</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>34</v>
@@ -2874,16 +3068,16 @@
       <c r="H34" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="9" t="s">
-        <v>35</v>
+      <c r="I34" t="s">
+        <v>216</v>
       </c>
       <c r="J34" s="11"/>
       <c r="K34" s="12">
-        <v>0.125</v>
+        <v>0.223</v>
       </c>
       <c r="L34" s="30">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.66900000000000004</v>
       </c>
       <c r="M34" s="31">
         <f>IF(OR(D34="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D34)</f>
@@ -2891,7 +3085,7 @@
       </c>
       <c r="N34" s="30">
         <f>IF(OR(L34="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L34)</f>
-        <v>13.125</v>
+        <v>23.415000000000003</v>
       </c>
       <c r="O34" s="10" t="s">
         <v>173</v>
@@ -3114,7 +3308,7 @@
       <c r="B40" s="33"/>
       <c r="C40" s="33"/>
       <c r="D40" s="8">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>60</v>
@@ -3128,24 +3322,24 @@
       <c r="H40" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="9" t="s">
-        <v>63</v>
+      <c r="I40" t="s">
+        <v>210</v>
       </c>
       <c r="J40" s="11"/>
       <c r="K40" s="12">
-        <v>0.108</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="L40" s="30">
         <f t="shared" si="0"/>
-        <v>0.432</v>
+        <v>1.7599999999999998</v>
       </c>
       <c r="M40" s="31">
         <f>IF(OR(D40="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D40)</f>
-        <v>140</v>
+        <v>700</v>
       </c>
       <c r="N40" s="30">
         <f>IF(OR(L40="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L40)</f>
-        <v>15.12</v>
+        <v>61.599999999999994</v>
       </c>
       <c r="O40" s="10" t="s">
         <v>173</v>
@@ -3379,16 +3573,16 @@
       <c r="H46" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I46" s="9" t="s">
-        <v>23</v>
+      <c r="I46" t="s">
+        <v>206</v>
       </c>
       <c r="J46" s="11"/>
       <c r="K46" s="12">
-        <v>0.01</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="L46" s="30">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.21999999999999997</v>
       </c>
       <c r="M46" s="31">
         <f>IF(OR(D46="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D46)</f>
@@ -3396,7 +3590,7 @@
       </c>
       <c r="N46" s="30">
         <f>IF(OR(L46="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L46)</f>
-        <v>7</v>
+        <v>7.6999999999999993</v>
       </c>
       <c r="O46" s="10" t="s">
         <v>173</v>
@@ -3404,7 +3598,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
@@ -3412,13 +3606,13 @@
         <v>1</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H47" s="33" t="s">
         <v>120</v>
@@ -3427,7 +3621,7 @@
         <v>2407171</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="K47" s="12">
         <v>55.64</v>
@@ -3450,7 +3644,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
@@ -3458,20 +3652,20 @@
         <v>2</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="G48" s="17"/>
       <c r="H48" s="33" t="s">
         <v>140</v>
       </c>
       <c r="I48" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="K48" s="18">
         <v>0.69</v>
@@ -3494,7 +3688,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
@@ -3502,20 +3696,20 @@
         <v>1</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F49" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="33" t="s">
         <v>140</v>
       </c>
       <c r="I49" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K49" s="12">
         <f>33/30.8*0.1</f>
@@ -3539,7 +3733,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
@@ -3547,20 +3741,20 @@
         <v>1</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F50" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="G50" s="10"/>
       <c r="H50" s="33" t="s">
         <v>145</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="K50" s="12">
         <v>1.24</v>
@@ -28260,33 +28454,33 @@
     <sortCondition ref="D1:D999"/>
   </sortState>
   <conditionalFormatting sqref="A2:B5 A7:B11 A13:B999">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="39" priority="9">
       <formula>(ISBLANK(A2)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O11 O13:O999">
-    <cfRule type="notContainsText" dxfId="14" priority="7" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="38" priority="7" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="36" priority="6">
       <formula>(ISBLANK(A12)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="notContainsText" dxfId="11" priority="4" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="35" priority="4" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O12))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>(ISBLANK(A6)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28307,7 +28501,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28329,7 +28523,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(Stückliste!L2:L999)</f>
-        <v>148.50614285714289</v>
+        <v>146.7471428571429</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -28339,7 +28533,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUM(Stückliste!N2:N999)</f>
-        <v>5197.7150000000001</v>
+        <v>5136.1499999999996</v>
       </c>
     </row>
   </sheetData>
@@ -28352,7 +28546,7 @@
   <dimension ref="A1:O999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28449,9 +28643,7 @@
         <f>IF(OR(L2="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L2)</f>
         <v/>
       </c>
-      <c r="O2" s="22" t="s">
-        <v>173</v>
-      </c>
+      <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -28493,9 +28685,7 @@
         <f>IF(OR(L3="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L3)</f>
         <v/>
       </c>
-      <c r="O3" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
@@ -28537,9 +28727,7 @@
         <f>IF(OR(L4="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L4)</f>
         <v/>
       </c>
-      <c r="O4" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -28579,13 +28767,11 @@
         <f>IF(OR(L5="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L5)</f>
         <v/>
       </c>
-      <c r="O5" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -28623,9 +28809,7 @@
         <f>IF(OR(L6="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L6)</f>
         <v/>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
@@ -28667,13 +28851,11 @@
         <f>IF(OR(L7="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L7)</f>
         <v/>
       </c>
-      <c r="O7" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -28705,13 +28887,11 @@
         <f>IF(OR(L8="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L8)</f>
         <v/>
       </c>
-      <c r="O8" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O8" s="10"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
@@ -28722,7 +28902,7 @@
         <v>67</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>22</v>
@@ -28749,13 +28929,11 @@
         <f>IF(OR(L9="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L9)</f>
         <v/>
       </c>
-      <c r="O9" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -28791,13 +28969,11 @@
         <f>IF(OR(L10="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L10)</f>
         <v/>
       </c>
-      <c r="O10" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
@@ -28835,13 +29011,11 @@
         <f>IF(OR(L11="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L11)</f>
         <v/>
       </c>
-      <c r="O11" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O11" s="10"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="33"/>
@@ -28877,232 +29051,348 @@
         <f>IF(OR(L12="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L12)</f>
         <v/>
       </c>
-      <c r="O12" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O12" s="10"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="30" t="str">
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="12">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="L13" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M13" s="31" t="str">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="M13" s="31">
         <f>IF(OR(D13="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D13)</f>
-        <v/>
-      </c>
-      <c r="N13" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N13" s="30">
         <f>IF(OR(L13="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L13)</f>
-        <v/>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>186</v>
-      </c>
+        <v>10.324999999999999</v>
+      </c>
+      <c r="O13" s="10"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+      <c r="A14" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B14" s="33"/>
       <c r="C14" s="33"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="30" t="str">
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="L14" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M14" s="31" t="str">
+        <v>0.375</v>
+      </c>
+      <c r="M14" s="31">
         <f>IF(OR(D14="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D14)</f>
-        <v/>
-      </c>
-      <c r="N14" s="30" t="str">
+        <v>105</v>
+      </c>
+      <c r="N14" s="30">
         <f>IF(OR(L14="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L14)</f>
-        <v/>
+        <v>13.125</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+      <c r="A15" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="9"/>
+      <c r="D15" s="8">
+        <v>20</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J15" s="11"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="30" t="str">
+      <c r="K15" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="L15" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M15" s="31" t="str">
+        <v>0.2</v>
+      </c>
+      <c r="M15" s="31">
         <f>IF(OR(D15="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D15)</f>
-        <v/>
-      </c>
-      <c r="N15" s="30" t="str">
+        <v>700</v>
+      </c>
+      <c r="N15" s="30">
         <f>IF(OR(L15="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L15)</f>
-        <v/>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+        <v>7</v>
+      </c>
+      <c r="O15" s="10"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="30" t="str">
+      <c r="H16" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16" s="9">
+        <v>632917</v>
+      </c>
+      <c r="J16" s="33"/>
+      <c r="K16" s="12">
+        <v>0.879</v>
+      </c>
+      <c r="L16" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M16" s="31" t="str">
+        <v>0.879</v>
+      </c>
+      <c r="M16" s="31">
         <f>IF(OR(D16="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D16)</f>
-        <v/>
-      </c>
-      <c r="N16" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N16" s="30">
         <f>IF(OR(L16="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L16)</f>
-        <v/>
+        <v>30.765000000000001</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="9"/>
+      <c r="D17" s="8">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="J17" s="11"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="30" t="str">
+      <c r="K17" s="12">
+        <v>0.108</v>
+      </c>
+      <c r="L17" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M17" s="31" t="str">
+        <v>0.432</v>
+      </c>
+      <c r="M17" s="31">
         <f>IF(OR(D17="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D17)</f>
-        <v/>
-      </c>
-      <c r="N17" s="30" t="str">
+        <v>140</v>
+      </c>
+      <c r="N17" s="30">
         <f>IF(OR(L17="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L17)</f>
-        <v/>
-      </c>
-      <c r="O17" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+        <v>15.12</v>
+      </c>
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="30" t="str">
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="12">
+        <v>16.57</v>
+      </c>
+      <c r="L18" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M18" s="31" t="str">
+        <v>16.57</v>
+      </c>
+      <c r="M18" s="31">
         <f>IF(OR(D18="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D18)</f>
-        <v/>
-      </c>
-      <c r="N18" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N18" s="30">
         <f>IF(OR(L18="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L18)</f>
-        <v/>
-      </c>
-      <c r="O18" s="10" t="s">
-        <v>180</v>
-      </c>
+        <v>579.95000000000005</v>
+      </c>
+      <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="30" t="str">
+      <c r="A19" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="20">
+        <v>1</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="I19" s="21">
+        <v>17390099</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="23">
+        <v>0.32</v>
+      </c>
+      <c r="L19" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M19" s="31" t="str">
+        <v>0.32</v>
+      </c>
+      <c r="M19" s="31">
         <f>IF(OR(D19="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D19)</f>
-        <v/>
-      </c>
-      <c r="N19" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N19" s="32">
         <f>IF(OR(L19="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L19)</f>
-        <v/>
+        <v>11.200000000000001</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="33" t="s">
+        <v>204</v>
+      </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="30" t="str">
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="12">
+        <v>1.62</v>
+      </c>
+      <c r="L20" s="30">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M20" s="31" t="str">
+        <v>1.62</v>
+      </c>
+      <c r="M20" s="31">
         <f>IF(OR(D20="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D20)</f>
-        <v/>
-      </c>
-      <c r="N20" s="30" t="str">
+        <v>35</v>
+      </c>
+      <c r="N20" s="30">
         <f>IF(OR(L20="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L20)</f>
-        <v/>
+        <v>56.7</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -29129,9 +29419,7 @@
         <f>IF(OR(L21="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L21)</f>
         <v/>
       </c>
-      <c r="O21" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O21" s="10"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
@@ -29157,9 +29445,7 @@
         <f>IF(OR(L22="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L22)</f>
         <v/>
       </c>
-      <c r="O22" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O22" s="10"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
@@ -29185,9 +29471,7 @@
         <f>IF(OR(L23="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L23)</f>
         <v/>
       </c>
-      <c r="O23" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O23" s="10"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
@@ -29213,9 +29497,7 @@
         <f>IF(OR(L24="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L24)</f>
         <v/>
       </c>
-      <c r="O24" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O24" s="10"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="33"/>
@@ -29241,9 +29523,7 @@
         <f>IF(OR(L25="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L25)</f>
         <v/>
       </c>
-      <c r="O25" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O25" s="10"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
@@ -29269,9 +29549,7 @@
         <f>IF(OR(L26="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L26)</f>
         <v/>
       </c>
-      <c r="O26" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O26" s="10"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
@@ -29297,9 +29575,7 @@
         <f>IF(OR(L27="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L27)</f>
         <v/>
       </c>
-      <c r="O27" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O27" s="10"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
@@ -29325,9 +29601,7 @@
         <f>IF(OR(L28="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L28)</f>
         <v/>
       </c>
-      <c r="O28" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O28" s="10"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
@@ -29353,9 +29627,7 @@
         <f>IF(OR(L29="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L29)</f>
         <v/>
       </c>
-      <c r="O29" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O29" s="10"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
@@ -29381,9 +29653,7 @@
         <f>IF(OR(L30="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L30)</f>
         <v/>
       </c>
-      <c r="O30" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O30" s="10"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
@@ -29409,9 +29679,7 @@
         <f>IF(OR(L31="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L31)</f>
         <v/>
       </c>
-      <c r="O31" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O31" s="10"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
@@ -29437,9 +29705,7 @@
         <f>IF(OR(L32="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L32)</f>
         <v/>
       </c>
-      <c r="O32" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O32" s="10"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
@@ -29465,9 +29731,7 @@
         <f>IF(OR(L33="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L33)</f>
         <v/>
       </c>
-      <c r="O33" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O33" s="10"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="33"/>
@@ -29493,9 +29757,7 @@
         <f>IF(OR(L34="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L34)</f>
         <v/>
       </c>
-      <c r="O34" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O34" s="10"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
@@ -29521,9 +29783,7 @@
         <f>IF(OR(L35="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L35)</f>
         <v/>
       </c>
-      <c r="O35" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O35" s="10"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
@@ -29549,9 +29809,7 @@
         <f>IF(OR(L36="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L36)</f>
         <v/>
       </c>
-      <c r="O36" s="10" t="s">
-        <v>187</v>
-      </c>
+      <c r="O36" s="10"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
@@ -29577,9 +29835,7 @@
         <f>IF(OR(L37="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L37)</f>
         <v/>
       </c>
-      <c r="O37" s="10" t="s">
-        <v>176</v>
-      </c>
+      <c r="O37" s="10"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="33"/>
@@ -29605,9 +29861,7 @@
         <f>IF(OR(L38="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L38)</f>
         <v/>
       </c>
-      <c r="O38" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O38" s="10"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="33"/>
@@ -29633,9 +29887,7 @@
         <f>IF(OR(L39="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L39)</f>
         <v/>
       </c>
-      <c r="O39" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O39" s="10"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="33"/>
@@ -29661,9 +29913,7 @@
         <f>IF(OR(L40="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L40)</f>
         <v/>
       </c>
-      <c r="O40" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O40" s="10"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="33"/>
@@ -29689,9 +29939,7 @@
         <f>IF(OR(L41="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L41)</f>
         <v/>
       </c>
-      <c r="O41" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O41" s="10"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="33"/>
@@ -29717,9 +29965,7 @@
         <f>IF(OR(L42="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L42)</f>
         <v/>
       </c>
-      <c r="O42" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O42" s="10"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="33"/>
@@ -29745,9 +29991,7 @@
         <f>IF(OR(L43="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L43)</f>
         <v/>
       </c>
-      <c r="O43" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O43" s="10"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="33"/>
@@ -29773,9 +30017,7 @@
         <f>IF(OR(L44="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L44)</f>
         <v/>
       </c>
-      <c r="O44" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O44" s="10"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="33"/>
@@ -29801,9 +30043,7 @@
         <f>IF(OR(L45="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L45)</f>
         <v/>
       </c>
-      <c r="O45" s="10" t="s">
-        <v>179</v>
-      </c>
+      <c r="O45" s="10"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="33"/>
@@ -29829,9 +30069,7 @@
         <f>IF(OR(L46="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L46)</f>
         <v/>
       </c>
-      <c r="O46" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O46" s="10"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="33"/>
@@ -29857,9 +30095,7 @@
         <f>IF(OR(L47="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L47)</f>
         <v/>
       </c>
-      <c r="O47" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O47" s="10"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="33"/>
@@ -29885,9 +30121,7 @@
         <f>IF(OR(L48="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L48)</f>
         <v/>
       </c>
-      <c r="O48" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O48" s="10"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
@@ -29913,9 +30147,7 @@
         <f>IF(OR(L49="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L49)</f>
         <v/>
       </c>
-      <c r="O49" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O49" s="10"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="33"/>
@@ -29941,9 +30173,7 @@
         <f>IF(OR(L50="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L50)</f>
         <v/>
       </c>
-      <c r="O50" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O50" s="10"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="33"/>
@@ -29969,9 +30199,7 @@
         <f>IF(OR(L51="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L51)</f>
         <v/>
       </c>
-      <c r="O51" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O51" s="10"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="33"/>
@@ -29997,9 +30225,7 @@
         <f>IF(OR(L52="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L52)</f>
         <v/>
       </c>
-      <c r="O52" s="10" t="s">
-        <v>188</v>
-      </c>
+      <c r="O52" s="10"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="33"/>
@@ -30025,9 +30251,7 @@
         <f>IF(OR(L53="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L53)</f>
         <v/>
       </c>
-      <c r="O53" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O53" s="10"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="33"/>
@@ -30053,9 +30277,7 @@
         <f>IF(OR(L54="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L54)</f>
         <v/>
       </c>
-      <c r="O54" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O54" s="10"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="33"/>
@@ -30081,9 +30303,7 @@
         <f>IF(OR(L55="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L55)</f>
         <v/>
       </c>
-      <c r="O55" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O55" s="10"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="33"/>
@@ -30109,9 +30329,7 @@
         <f>IF(OR(L56="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L56)</f>
         <v/>
       </c>
-      <c r="O56" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O56" s="10"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="33"/>
@@ -30137,9 +30355,7 @@
         <f>IF(OR(L57="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L57)</f>
         <v/>
       </c>
-      <c r="O57" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="O57" s="10"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="33"/>
@@ -54634,43 +54850,147 @@
       <c r="O999" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:B5 A13:B999 A7:B11">
-    <cfRule type="expression" dxfId="8" priority="9">
+  <conditionalFormatting sqref="A2:B5 A21:B999 A7:B11">
+    <cfRule type="expression" dxfId="32" priority="33">
       <formula>(ISBLANK(A2)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O5 O13:O999 O7:O11">
-    <cfRule type="notContainsText" dxfId="7" priority="7" operator="notContains" text="ok">
+  <conditionalFormatting sqref="O2:O5 O21:O999 O7:O11">
+    <cfRule type="notContainsText" dxfId="31" priority="31" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>(ISBLANK(A12)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="28" priority="28" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O12))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="ok">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="ok">
       <formula>NOT(ISERROR(SEARCH("ok",O12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>(ISBLANK(A6)=FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="notContainsText" dxfId="1" priority="1" operator="notContains" text="ok">
+    <cfRule type="notContainsText" dxfId="25" priority="25" operator="notContains" text="ok">
       <formula>ISERROR(SEARCH("ok",O6))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O13">
+    <cfRule type="notContainsText" dxfId="23" priority="23" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O13))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13:B13">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>(ISBLANK(A13)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:B14">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>(ISBLANK(A14)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14">
+    <cfRule type="notContainsText" dxfId="19" priority="19" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O14))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:B15">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>(ISBLANK(A15)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15">
+    <cfRule type="notContainsText" dxfId="16" priority="16" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O15))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16:B16">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>(ISBLANK(A16)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O16">
+    <cfRule type="notContainsText" dxfId="13" priority="13" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O16))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:B17">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>(ISBLANK(A17)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="notContainsText" dxfId="10" priority="10" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O17))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B18">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>(ISBLANK(A18)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
+    <cfRule type="notContainsText" dxfId="7" priority="7" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O18))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:B19">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>(ISBLANK(A19)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O19">
+    <cfRule type="notContainsText" dxfId="4" priority="4" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O19))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="ok">
+      <formula>NOT(ISERROR(SEARCH("ok",O19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:B20">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>(ISBLANK(A20)=FALSE)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20">
+    <cfRule type="notContainsText" dxfId="1" priority="1" operator="notContains" text="ok">
+      <formula>ISERROR(SEARCH("ok",O20))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ok">
-      <formula>NOT(ISERROR(SEARCH("ok",O6)))</formula>
+      <formula>NOT(ISERROR(SEARCH("ok",O20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LED Helligkeit mit einstellbarem PWM
</commit_message>
<xml_diff>
--- a/BOM/materialliste_microcontroller_board.xlsx
+++ b/BOM/materialliste_microcontroller_board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uC_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09159A4-A436-4E4F-9456-E30FF383FF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B41013-0EBC-486D-B602-14C3E6EEAD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="278">
   <si>
     <t>Bemerkung</t>
   </si>
@@ -870,6 +870,42 @@
   </si>
   <si>
     <t>Zeit Board 2</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>shotky</t>
+  </si>
+  <si>
+    <t>SOD-123-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-SD103CW-HE3_A-08 </t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Vishay/SD103CW-HE3_A-08?qs=Imq1NPwxi75eP9XDj9IIZg%3D%3D</t>
+  </si>
+  <si>
+    <t>Kondensator</t>
+  </si>
+  <si>
+    <t>22nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-CC805JRX7R8BB223 </t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/YAGEO/CC0805JRX7R8BB223?qs=57cj7OiSijk%252BueqZYCThQQ%3D%3D</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-CR0805JW-471ELF </t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/Bourns/CR0805-JW-471ELF?qs=sGAEpiMZZMukHu%252BjC5l7YeTlYklQq7xRXmy1WbvLzUg%3D</t>
   </si>
 </sst>
 </file>
@@ -1959,7 +1995,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,7 +3415,7 @@
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
       <c r="D31" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>68</v>
@@ -3400,15 +3436,15 @@
       </c>
       <c r="L31" s="29">
         <f t="shared" si="0"/>
-        <v>1.62</v>
+        <v>3.24</v>
       </c>
       <c r="M31" s="30">
         <f>IF(OR(D31="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D31)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="N31" s="29">
         <f>IF(OR(L31="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L31)</f>
-        <v>64.800000000000011</v>
+        <v>129.60000000000002</v>
       </c>
       <c r="O31" s="9">
         <v>80</v>
@@ -3416,7 +3452,7 @@
       <c r="P31" s="9"/>
       <c r="Q31" s="59">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -4130,7 +4166,7 @@
       <c r="B47" s="32"/>
       <c r="C47" s="32"/>
       <c r="D47" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>168</v>
@@ -4153,15 +4189,15 @@
       </c>
       <c r="L47" s="29">
         <f t="shared" si="0"/>
-        <v>1.7599999999999998</v>
+        <v>1.8479999999999999</v>
       </c>
       <c r="M47" s="30">
         <f>IF(OR(D47="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D47)</f>
-        <v>800</v>
+        <v>840</v>
       </c>
       <c r="N47" s="29">
         <f>IF(OR(L47="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L47)</f>
-        <v>70.399999999999991</v>
+        <v>73.919999999999987</v>
       </c>
       <c r="O47" s="9">
         <v>400</v>
@@ -4169,7 +4205,7 @@
       <c r="P47" s="9"/>
       <c r="Q47" s="59">
         <f t="shared" si="1"/>
-        <v>-400</v>
+        <v>-440</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -4460,90 +4496,138 @@
       <c r="A54" s="32"/>
       <c r="B54" s="32"/>
       <c r="C54" s="32"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="29" t="str">
+      <c r="D54" s="8">
+        <v>2</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="H54" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I54" t="s">
+        <v>269</v>
+      </c>
+      <c r="J54" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="K54" s="18">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="L54" s="29">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M54" s="30" t="str">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="M54" s="30">
         <f>IF(OR(D54="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D54)</f>
-        <v/>
-      </c>
-      <c r="N54" s="29" t="str">
+        <v>80</v>
+      </c>
+      <c r="N54" s="29">
         <f>IF(OR(L54="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L54)</f>
-        <v/>
+        <v>19.28</v>
       </c>
       <c r="P54" s="9"/>
-      <c r="Q54" s="59" t="e">
+      <c r="Q54" s="59">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="32"/>
       <c r="B55" s="32"/>
       <c r="C55" s="32"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="29" t="str">
+      <c r="D55" s="8">
+        <v>1</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H55" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I55" t="s">
+        <v>273</v>
+      </c>
+      <c r="J55" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="K55" s="18">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L55" s="29">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M55" s="30" t="str">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M55" s="30">
         <f>IF(OR(D55="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D55)</f>
-        <v/>
-      </c>
-      <c r="N55" s="29" t="str">
+        <v>40</v>
+      </c>
+      <c r="N55" s="29">
         <f>IF(OR(L55="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L55)</f>
-        <v/>
+        <v>1.92</v>
       </c>
       <c r="P55" s="9"/>
-      <c r="Q55" s="59" t="e">
+      <c r="Q55" s="59">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="32"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="9"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="29" t="str">
+      <c r="D56" s="8">
+        <v>2</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H56" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I56" t="s">
+        <v>276</v>
+      </c>
+      <c r="J56" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="K56" s="18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L56" s="29">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M56" s="30" t="str">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M56" s="30">
         <f>IF(OR(D56="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D56)</f>
-        <v/>
-      </c>
-      <c r="N56" s="29" t="str">
+        <v>80</v>
+      </c>
+      <c r="N56" s="29">
         <f>IF(OR(L56="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L56)</f>
-        <v/>
+        <v>0.87999999999999989</v>
       </c>
       <c r="P56" s="9"/>
-      <c r="Q56" s="59" t="e">
+      <c r="Q56" s="59">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -29695,7 +29779,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(Stückliste!L2:L999)</f>
-        <v>106.93914285714284</v>
+        <v>109.19914285714283</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -29705,7 +29789,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUM(Stückliste!N2:N999)</f>
-        <v>4277.5657142857135</v>
+        <v>4367.9657142857131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5.1kR Widerstände in BOM und Kommentar in Schema gelöscht
</commit_message>
<xml_diff>
--- a/BOM/materialliste_microcontroller_board.xlsx
+++ b/BOM/materialliste_microcontroller_board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uC_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B41013-0EBC-486D-B602-14C3E6EEAD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012F6E32-2D3E-4250-A3C4-D1620670F68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DEAA252D-CCA8-493C-A99A-AAF8A4EEE89B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="281">
   <si>
     <t>Bemerkung</t>
   </si>
@@ -906,6 +906,15 @@
   </si>
   <si>
     <t>https://www.mouser.ch/ProductDetail/Bourns/CR0805-JW-471ELF?qs=sGAEpiMZZMukHu%252BjC5l7YeTlYklQq7xRXmy1WbvLzUg%3D</t>
+  </si>
+  <si>
+    <t>5k1R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">755-SFR10EZPF5101 </t>
+  </si>
+  <si>
+    <t>https://www.mouser.ch/ProductDetail/ROHM-Semiconductor/SFR10EZPF5101?qs=PqoDHHvF6491bPJygeZFGw%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -1994,8 +2003,8 @@
   <dimension ref="A1:Q999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,30 +4643,46 @@
       <c r="A57" s="32"/>
       <c r="B57" s="32"/>
       <c r="C57" s="32"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="29" t="str">
+      <c r="D57" s="8">
+        <v>2</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H57" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I57" t="s">
+        <v>279</v>
+      </c>
+      <c r="J57" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="K57" s="18">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="L57" s="29">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M57" s="30" t="str">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="M57" s="30">
         <f>IF(OR(D57="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*D57)</f>
-        <v/>
-      </c>
-      <c r="N57" s="29" t="str">
+        <v>80</v>
+      </c>
+      <c r="N57" s="29">
         <f>IF(OR(L57="",'Anzahl &amp; Preis'!$B$1=""),"",'Anzahl &amp; Preis'!$B$1*L57)</f>
-        <v/>
+        <v>10.56</v>
       </c>
       <c r="P57" s="9"/>
-      <c r="Q57" s="59" t="e">
+      <c r="Q57" s="59">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -29779,7 +29804,7 @@
       </c>
       <c r="B2" s="4">
         <f>SUM(Stückliste!L2:L999)</f>
-        <v>109.19914285714283</v>
+        <v>109.46314285714283</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -29789,7 +29814,7 @@
       </c>
       <c r="B3" s="6">
         <f>SUM(Stückliste!N2:N999)</f>
-        <v>4367.9657142857131</v>
+        <v>4378.5257142857135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>